<commit_message>
* invitation task: correct response added in schedule for module 2b
</commit_message>
<xml_diff>
--- a/public/js/tasks/invitation_task/MCQ_mapping_module3-1.xlsx
+++ b/public/js/tasks/invitation_task/MCQ_mapping_module3-1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jtouthang/iCloud Drive (Archive)/Documents/Documents - L00019188/StimTool_Online/public/js/tasks/invitation_task/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3F8A91-2A42-E641-8813-7506CF103BB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7053FADA-8476-D448-B667-5840B4D86308}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21480" windowHeight="14940" xr2:uid="{193BAE17-2DD3-4B9C-A546-95C76A9087F0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="68800" windowHeight="28300" xr2:uid="{193BAE17-2DD3-4B9C-A546-95C76A9087F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="31">
   <si>
     <t>building_type</t>
   </si>
@@ -119,10 +119,13 @@
     <t>5-2</t>
   </si>
   <si>
+    <t>correct</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
     <t>left</t>
-  </si>
-  <si>
-    <t>right</t>
   </si>
 </sst>
 </file>
@@ -475,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E664A047-A8AA-4A90-B33E-4BBE354FFB25}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="AF25" sqref="AF25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -488,7 +491,7 @@
     <col min="5" max="8" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -513,8 +516,11 @@
       <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -525,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>15</v>
@@ -539,8 +545,11 @@
       <c r="H2" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -565,8 +574,11 @@
       <c r="H3" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -577,22 +589,25 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -617,8 +632,11 @@
       <c r="H5" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -629,7 +647,7 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>15</v>
@@ -643,8 +661,11 @@
       <c r="H6" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -669,8 +690,11 @@
       <c r="H7" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -681,7 +705,7 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>13</v>
@@ -695,8 +719,11 @@
       <c r="H8" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -721,8 +748,11 @@
       <c r="H9" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -733,7 +763,7 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>22</v>
@@ -747,8 +777,11 @@
       <c r="H10" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -773,8 +806,11 @@
       <c r="H11" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -785,22 +821,25 @@
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -825,8 +864,11 @@
       <c r="H13" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -837,7 +879,7 @@
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>13</v>
@@ -851,8 +893,11 @@
       <c r="H14" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -866,10 +911,10 @@
         <v>29</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>17</v>
@@ -877,8 +922,11 @@
       <c r="H15" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -889,7 +937,7 @@
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>19</v>
@@ -903,8 +951,11 @@
       <c r="H16" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -929,8 +980,11 @@
       <c r="H17" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -941,7 +995,7 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>25</v>
@@ -955,8 +1009,11 @@
       <c r="H18" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -981,8 +1038,11 @@
       <c r="H19" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -993,7 +1053,7 @@
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>25</v>
@@ -1007,8 +1067,11 @@
       <c r="H20" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -1033,8 +1096,11 @@
       <c r="H21" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -1045,7 +1111,7 @@
         <v>6</v>
       </c>
       <c r="D22" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>16</v>
@@ -1059,8 +1125,11 @@
       <c r="H22" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -1085,8 +1154,11 @@
       <c r="H23" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -1097,7 +1169,7 @@
         <v>6</v>
       </c>
       <c r="D24" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>19</v>
@@ -1111,8 +1183,11 @@
       <c r="H24" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -1137,8 +1212,11 @@
       <c r="H25" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -1149,7 +1227,7 @@
         <v>7</v>
       </c>
       <c r="D26" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>21</v>
@@ -1163,8 +1241,11 @@
       <c r="H26" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -1184,13 +1265,16 @@
         <v>25</v>
       </c>
       <c r="G27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H27" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -1201,7 +1285,7 @@
         <v>7</v>
       </c>
       <c r="D28" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>14</v>
@@ -1215,8 +1299,11 @@
       <c r="H28" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>2</v>
       </c>
@@ -1240,13 +1327,16 @@
       </c>
       <c r="H29" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="F2 G3 F5 F8 E7 F9:G11 F12:G17 E12 E18:H23 H12 E13:E17 H13:H17 E24:H29" twoDigitTextYear="1"/>
+    <ignoredError sqref="F2 G3 F5 F8 E7 F9:G11 F13:G14 E18:H23 H12 E13:E14 H13:H17 E24:H26 F12 E16:E17 F16:G17 G15 E28:H29 E27:F27" twoDigitTextYear="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
* invitation task: used different path versions
</commit_message>
<xml_diff>
--- a/public/js/tasks/invitation_task/MCQ_mapping_module3-1.xlsx
+++ b/public/js/tasks/invitation_task/MCQ_mapping_module3-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jtouthang/iCloud Drive (Archive)/Documents/Documents - L00019188/StimTool_Online/public/js/tasks/invitation_task/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7053FADA-8476-D448-B667-5840B4D86308}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35D4412-84BF-364B-9D83-99AD4808D28D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="68800" windowHeight="28300" xr2:uid="{193BAE17-2DD3-4B9C-A546-95C76A9087F0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="32">
   <si>
     <t>building_type</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>left</t>
+  </si>
+  <si>
+    <t>path_version</t>
   </si>
 </sst>
 </file>
@@ -478,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E664A047-A8AA-4A90-B33E-4BBE354FFB25}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF25" sqref="AF25"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -489,9 +492,10 @@
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
     <col min="5" max="8" width="8.6640625" style="1"/>
+    <col min="10" max="10" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -519,8 +523,11 @@
       <c r="I1" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -548,8 +555,11 @@
       <c r="I2" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -577,8 +587,11 @@
       <c r="I3" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -606,8 +619,11 @@
       <c r="I4" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -635,8 +651,11 @@
       <c r="I5" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -664,8 +683,11 @@
       <c r="I6" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -693,8 +715,11 @@
       <c r="I7" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -722,8 +747,11 @@
       <c r="I8" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -751,8 +779,11 @@
       <c r="I9" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -780,8 +811,11 @@
       <c r="I10" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -809,8 +843,11 @@
       <c r="I11" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -838,8 +875,11 @@
       <c r="I12" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -867,8 +907,11 @@
       <c r="I13" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -896,8 +939,11 @@
       <c r="I14" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -925,8 +971,11 @@
       <c r="I15" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -954,8 +1003,11 @@
       <c r="I16" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -983,8 +1035,11 @@
       <c r="I17" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -1012,8 +1067,11 @@
       <c r="I18" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -1041,8 +1099,11 @@
       <c r="I19" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -1070,8 +1131,11 @@
       <c r="I20" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -1099,8 +1163,11 @@
       <c r="I21" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -1128,8 +1195,11 @@
       <c r="I22" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -1157,8 +1227,11 @@
       <c r="I23" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -1186,8 +1259,11 @@
       <c r="I24" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -1215,8 +1291,11 @@
       <c r="I25" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -1244,8 +1323,11 @@
       <c r="I26" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -1273,8 +1355,11 @@
       <c r="I27" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -1302,8 +1387,11 @@
       <c r="I28" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>2</v>
       </c>
@@ -1330,6 +1418,9 @@
       </c>
       <c r="I29" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Invitation: Replaced building images. Implemented accept and reject blocks in module 1. Added break switch slides. Implemented score bar and score value pop-up. Changed upper right trial count to be out of block total instead of module total.
</commit_message>
<xml_diff>
--- a/public/js/tasks/invitation_task/MCQ_mapping_module3-1.xlsx
+++ b/public/js/tasks/invitation_task/MCQ_mapping_module3-1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jtouthang/iCloud Drive (Archive)/Documents/Documents - L00019188/StimTool_Online/public/js/tasks/invitation_task/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ARobinson\Documents\stimtool\stimtool_schedules\invitation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35D4412-84BF-364B-9D83-99AD4808D28D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B24FC8D-A5F1-4771-A8C8-678D735DE548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="68800" windowHeight="28300" xr2:uid="{193BAE17-2DD3-4B9C-A546-95C76A9087F0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="16200" xr2:uid="{193BAE17-2DD3-4B9C-A546-95C76A9087F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="34">
   <si>
     <t>building_type</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>path_version</t>
+  </si>
+  <si>
+    <t>20-20</t>
+  </si>
+  <si>
+    <t>10-25</t>
   </si>
 </sst>
 </file>
@@ -484,18 +490,18 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="5" max="8" width="8.6640625" style="1"/>
-    <col min="10" max="10" width="14.1640625" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="5" max="8" width="8.7109375" style="1"/>
+    <col min="10" max="10" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -527,7 +533,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -550,7 +556,7 @@
         <v>20</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>10</v>
@@ -559,7 +565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -579,7 +585,7 @@
         <v>17</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>15</v>
@@ -591,7 +597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -611,10 +617,10 @@
         <v>14</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>9</v>
@@ -623,7 +629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -637,7 +643,7 @@
         <v>29</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>16</v>
@@ -655,7 +661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -687,7 +693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -707,7 +713,7 @@
         <v>11</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>21</v>
@@ -719,7 +725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -736,7 +742,7 @@
         <v>13</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>14</v>
@@ -751,7 +757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -765,7 +771,7 @@
         <v>29</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>16</v>
@@ -783,7 +789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -800,7 +806,7 @@
         <v>22</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>21</v>
@@ -815,7 +821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -829,10 +835,10 @@
         <v>29</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>25</v>
@@ -847,7 +853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -861,13 +867,13 @@
         <v>30</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>16</v>
@@ -879,7 +885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -896,7 +902,7 @@
         <v>18</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>16</v>
@@ -911,7 +917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -934,7 +940,7 @@
         <v>18</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>10</v>
@@ -943,7 +949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -960,10 +966,10 @@
         <v>19</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>12</v>
@@ -975,7 +981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -995,7 +1001,7 @@
         <v>26</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>15</v>
@@ -1007,7 +1013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -1021,7 +1027,7 @@
         <v>29</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>17</v>
@@ -1039,7 +1045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -1071,7 +1077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -1091,7 +1097,7 @@
         <v>18</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>15</v>
@@ -1103,7 +1109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -1117,7 +1123,7 @@
         <v>30</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>13</v>
@@ -1135,7 +1141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -1155,7 +1161,7 @@
         <v>21</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>18</v>
@@ -1167,7 +1173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -1181,7 +1187,7 @@
         <v>30</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>15</v>
@@ -1199,7 +1205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -1213,7 +1219,7 @@
         <v>29</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>14</v>
@@ -1231,7 +1237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -1254,7 +1260,7 @@
         <v>21</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>10</v>
@@ -1263,7 +1269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -1277,7 +1283,7 @@
         <v>29</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>26</v>
@@ -1295,7 +1301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -1315,7 +1321,7 @@
         <v>20</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>15</v>
@@ -1327,7 +1333,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -1350,7 +1356,7 @@
         <v>14</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>10</v>
@@ -1359,7 +1365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -1373,10 +1379,10 @@
         <v>30</v>
       </c>
       <c r="E28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>20</v>
@@ -1391,7 +1397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>2</v>
       </c>
@@ -1405,7 +1411,7 @@
         <v>29</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>19</v>
@@ -1427,7 +1433,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="F2 G3 F5 F8 E7 F9:G11 F13:G14 E18:H23 H12 E13:E14 H13:H17 E24:H26 F12 E16:E17 F16:G17 G15 E28:H29 E27:F27" twoDigitTextYear="1"/>
+    <ignoredError sqref="F2 F5 E7 F9:G9 F14:G14 E18:H18 H12 E13:E14 H13 F25:H25 F12 E16 F17:G17 F29:H29 E27:F27 G11 G10 G13 H15:H17 F16 F23:H23 E19:F19 H19 F20:H20 E21:F21 H21 F22:H22 E26:F26 H26 E24:G24 G28:H28" twoDigitTextYear="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>